<commit_message>
.jar a mejorar y actualizacion totu
</commit_message>
<xml_diff>
--- a/software/functionalities/fun_1.xlsx
+++ b/software/functionalities/fun_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unavarra-my.sharepoint.com/personal/sola_146618_e_unavarra_es/Documents/Escritorio/PRACTICAS/VENTILADORES/funcionalidades/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unavarra-my.sharepoint.com/personal/sola_146618_e_unavarra_es/Documents/Escritorio/PRACTICAS/VENTILADORES/JavaFAWT/software/functionalities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{7C803FA5-91A8-499A-908A-C71DE79208F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86D516DC-5506-425D-B8A3-0EEB8940CB35}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{7C803FA5-91A8-499A-908A-C71DE79208F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D389504-E049-43BF-AF34-18606487D61B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6821E79B-E030-4E06-A8F5-5E441BDD30E2}"/>
   </bookViews>
@@ -37,8 +37,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -117,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -132,6 +140,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -151,14 +168,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -196,7 +209,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -302,7 +315,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -444,7 +457,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -452,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80804853-67A5-4695-984F-057822B8511A}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -837,40 +850,40 @@
         <v>3000</v>
       </c>
       <c r="B10" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C10" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D10" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E10" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F10" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G10" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H10" s="3">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I10" s="3">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="J10" s="3">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="K10" s="3">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="L10" s="3">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="M10" s="3">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -878,40 +891,40 @@
         <v>3000</v>
       </c>
       <c r="B11" s="2">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C11" s="2">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="D11" s="2">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E11" s="2">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F11" s="2">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G11" s="2">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="H11" s="3">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="I11" s="3">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="J11" s="3">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="K11" s="3">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="L11" s="3">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="M11" s="3">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -919,40 +932,40 @@
         <v>3000</v>
       </c>
       <c r="B12" s="2">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C12" s="2">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E12" s="2">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="F12" s="2">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="G12" s="2">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="H12" s="3">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="I12" s="3">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="J12" s="3">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="K12" s="3">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="L12" s="3">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="M12" s="3">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -960,40 +973,40 @@
         <v>3000</v>
       </c>
       <c r="B13" s="2">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C13" s="2">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="D13" s="2">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="E13" s="2">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F13" s="2">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="G13" s="2">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="H13" s="3">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="I13" s="3">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="J13" s="3">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="K13" s="3">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="L13" s="3">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="M13" s="3">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1001,40 +1014,40 @@
         <v>3000</v>
       </c>
       <c r="B14" s="2">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="E14" s="2">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="F14" s="2">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="G14" s="2">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="H14" s="3">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="I14" s="3">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="J14" s="3">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="K14" s="3">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="L14" s="3">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="M14" s="3">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1042,40 +1055,40 @@
         <v>3000</v>
       </c>
       <c r="B15" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="E15" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="F15" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G15" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H15" s="3">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I15" s="3">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="J15" s="3">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K15" s="3">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L15" s="3">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="M15" s="3">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1083,40 +1096,40 @@
         <v>3000</v>
       </c>
       <c r="B16" s="2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D16" s="2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E16" s="2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F16" s="2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G16" s="2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H16" s="3">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="I16" s="3">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="J16" s="3">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="K16" s="3">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="L16" s="3">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="M16" s="3">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1124,40 +1137,40 @@
         <v>3000</v>
       </c>
       <c r="B17" s="2">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D17" s="2">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E17" s="2">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="F17" s="2">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G17" s="2">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="H17" s="3">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="I17" s="3">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="J17" s="3">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="K17" s="3">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="L17" s="3">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="M17" s="3">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -1165,40 +1178,40 @@
         <v>3000</v>
       </c>
       <c r="B18" s="2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C18" s="2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E18" s="2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F18" s="2">
-        <v>30</v>
-      </c>
-      <c r="G18" s="2">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0</v>
       </c>
       <c r="H18" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I18" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J18" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K18" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="L18" s="3">
-        <v>30</v>
-      </c>
-      <c r="M18" s="3">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -1206,40 +1219,40 @@
         <v>3000</v>
       </c>
       <c r="B19" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C19" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E19" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F19" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G19" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H19" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I19" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J19" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K19" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L19" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="M19" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -1247,40 +1260,40 @@
         <v>3000</v>
       </c>
       <c r="B20" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C20" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D20" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E20" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F20" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G20" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H20" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I20" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J20" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K20" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L20" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M20" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -1288,40 +1301,40 @@
         <v>3000</v>
       </c>
       <c r="B21" s="2">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D21" s="2">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E21" s="2">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F21" s="2">
-        <v>0</v>
-      </c>
-      <c r="G21" s="5">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="G21" s="2">
+        <v>30</v>
       </c>
       <c r="H21" s="3">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I21" s="3">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J21" s="3">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K21" s="3">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L21" s="3">
-        <v>0</v>
-      </c>
-      <c r="M21" s="4">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="M21" s="3">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -1329,40 +1342,40 @@
         <v>3000</v>
       </c>
       <c r="B22" s="2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C22" s="2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D22" s="2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E22" s="2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F22" s="2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G22" s="2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="H22" s="3">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="I22" s="3">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="J22" s="3">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="K22" s="3">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="L22" s="3">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="M22" s="3">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -1370,40 +1383,40 @@
         <v>3000</v>
       </c>
       <c r="B23" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C23" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D23" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E23" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F23" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="G23" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H23" s="3">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="I23" s="3">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="J23" s="3">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="K23" s="3">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="L23" s="3">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="M23" s="3">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -1411,40 +1424,40 @@
         <v>3000</v>
       </c>
       <c r="B24" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C24" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D24" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E24" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F24" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G24" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H24" s="3">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="I24" s="3">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="J24" s="3">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K24" s="3">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="L24" s="3">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="M24" s="3">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -1452,40 +1465,40 @@
         <v>3000</v>
       </c>
       <c r="B25" s="2">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="C25" s="2">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D25" s="2">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E25" s="2">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="F25" s="2">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="G25" s="2">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="H25" s="3">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="I25" s="3">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="J25" s="3">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="K25" s="3">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="L25" s="3">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="M25" s="3">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -1493,163 +1506,163 @@
         <v>3000</v>
       </c>
       <c r="B26" s="2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C26" s="2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D26" s="2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="E26" s="2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F26" s="2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="G26" s="2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="H26" s="3">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="I26" s="3">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="J26" s="3">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="K26" s="3">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="L26" s="3">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="M26" s="3">
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>3000</v>
-      </c>
-      <c r="B27" s="2">
-        <v>60</v>
-      </c>
-      <c r="C27" s="2">
-        <v>60</v>
-      </c>
-      <c r="D27" s="2">
-        <v>60</v>
-      </c>
-      <c r="E27" s="2">
-        <v>60</v>
-      </c>
-      <c r="F27" s="2">
-        <v>60</v>
-      </c>
-      <c r="G27" s="2">
-        <v>60</v>
-      </c>
-      <c r="H27" s="3">
-        <v>60</v>
-      </c>
-      <c r="I27" s="3">
-        <v>60</v>
-      </c>
-      <c r="J27" s="3">
-        <v>60</v>
-      </c>
-      <c r="K27" s="3">
-        <v>60</v>
-      </c>
-      <c r="L27" s="3">
-        <v>60</v>
-      </c>
-      <c r="M27" s="3">
-        <v>60</v>
+      <c r="A27" s="6">
+        <v>3000</v>
+      </c>
+      <c r="B27" s="7">
+        <v>80</v>
+      </c>
+      <c r="C27" s="7">
+        <v>80</v>
+      </c>
+      <c r="D27" s="7">
+        <v>80</v>
+      </c>
+      <c r="E27" s="7">
+        <v>80</v>
+      </c>
+      <c r="F27" s="7">
+        <v>80</v>
+      </c>
+      <c r="G27" s="7">
+        <v>80</v>
+      </c>
+      <c r="H27" s="8">
+        <v>80</v>
+      </c>
+      <c r="I27" s="8">
+        <v>80</v>
+      </c>
+      <c r="J27" s="8">
+        <v>80</v>
+      </c>
+      <c r="K27" s="8">
+        <v>80</v>
+      </c>
+      <c r="L27" s="8">
+        <v>80</v>
+      </c>
+      <c r="M27" s="8">
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>3000</v>
-      </c>
-      <c r="B28" s="2">
-        <v>70</v>
-      </c>
-      <c r="C28" s="2">
-        <v>70</v>
-      </c>
-      <c r="D28" s="2">
-        <v>70</v>
-      </c>
-      <c r="E28" s="2">
-        <v>70</v>
-      </c>
-      <c r="F28" s="2">
-        <v>70</v>
-      </c>
-      <c r="G28" s="2">
-        <v>70</v>
-      </c>
-      <c r="H28" s="3">
-        <v>70</v>
-      </c>
-      <c r="I28" s="3">
-        <v>70</v>
-      </c>
-      <c r="J28" s="3">
-        <v>70</v>
-      </c>
-      <c r="K28" s="3">
-        <v>70</v>
-      </c>
-      <c r="L28" s="3">
-        <v>70</v>
-      </c>
-      <c r="M28" s="3">
+      <c r="A28" s="6">
+        <v>3000</v>
+      </c>
+      <c r="B28" s="7">
+        <v>70</v>
+      </c>
+      <c r="C28" s="7">
+        <v>70</v>
+      </c>
+      <c r="D28" s="7">
+        <v>70</v>
+      </c>
+      <c r="E28" s="7">
+        <v>70</v>
+      </c>
+      <c r="F28" s="7">
+        <v>70</v>
+      </c>
+      <c r="G28" s="7">
+        <v>70</v>
+      </c>
+      <c r="H28" s="8">
+        <v>70</v>
+      </c>
+      <c r="I28" s="8">
+        <v>70</v>
+      </c>
+      <c r="J28" s="8">
+        <v>70</v>
+      </c>
+      <c r="K28" s="8">
+        <v>70</v>
+      </c>
+      <c r="L28" s="8">
+        <v>70</v>
+      </c>
+      <c r="M28" s="8">
         <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>3000</v>
-      </c>
-      <c r="B29" s="2">
-        <v>80</v>
-      </c>
-      <c r="C29" s="2">
-        <v>80</v>
-      </c>
-      <c r="D29" s="2">
-        <v>80</v>
-      </c>
-      <c r="E29" s="2">
-        <v>80</v>
-      </c>
-      <c r="F29" s="2">
-        <v>80</v>
-      </c>
-      <c r="G29" s="2">
-        <v>80</v>
-      </c>
-      <c r="H29" s="3">
-        <v>80</v>
-      </c>
-      <c r="I29" s="3">
-        <v>80</v>
-      </c>
-      <c r="J29" s="3">
-        <v>80</v>
-      </c>
-      <c r="K29" s="3">
-        <v>80</v>
-      </c>
-      <c r="L29" s="3">
-        <v>80</v>
-      </c>
-      <c r="M29" s="3">
-        <v>80</v>
+      <c r="A29" s="6">
+        <v>3000</v>
+      </c>
+      <c r="B29" s="7">
+        <v>60</v>
+      </c>
+      <c r="C29" s="7">
+        <v>60</v>
+      </c>
+      <c r="D29" s="7">
+        <v>60</v>
+      </c>
+      <c r="E29" s="7">
+        <v>60</v>
+      </c>
+      <c r="F29" s="7">
+        <v>60</v>
+      </c>
+      <c r="G29" s="7">
+        <v>60</v>
+      </c>
+      <c r="H29" s="8">
+        <v>60</v>
+      </c>
+      <c r="I29" s="8">
+        <v>60</v>
+      </c>
+      <c r="J29" s="8">
+        <v>60</v>
+      </c>
+      <c r="K29" s="8">
+        <v>60</v>
+      </c>
+      <c r="L29" s="8">
+        <v>60</v>
+      </c>
+      <c r="M29" s="8">
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -1657,40 +1670,40 @@
         <v>3000</v>
       </c>
       <c r="B30" s="2">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="C30" s="2">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="D30" s="2">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="E30" s="2">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="F30" s="2">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G30" s="2">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="H30" s="3">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="I30" s="3">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="J30" s="3">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="K30" s="3">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="L30" s="3">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="M30" s="3">
-        <v>90</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -1698,40 +1711,40 @@
         <v>3000</v>
       </c>
       <c r="B31" s="2">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="C31" s="2">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="D31" s="2">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="E31" s="2">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="F31" s="2">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G31" s="2">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="H31" s="3">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="I31" s="3">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="J31" s="3">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="K31" s="3">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="L31" s="3">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M31" s="3">
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -1739,40 +1752,40 @@
         <v>3000</v>
       </c>
       <c r="B32" s="2">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="C32" s="2">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="D32" s="2">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="E32" s="2">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="F32" s="2">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="G32" s="2">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="H32" s="3">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="I32" s="3">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J32" s="3">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="K32" s="3">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="L32" s="3">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="M32" s="3">
-        <v>90</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -1780,40 +1793,40 @@
         <v>3000</v>
       </c>
       <c r="B33" s="2">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C33" s="2">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="D33" s="2">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="E33" s="2">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="F33" s="2">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="G33" s="2">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H33" s="3">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I33" s="3">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="J33" s="3">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="K33" s="3">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="L33" s="3">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="M33" s="3">
-        <v>80</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
@@ -1821,40 +1834,40 @@
         <v>3000</v>
       </c>
       <c r="B34" s="2">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C34" s="2">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="D34" s="2">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E34" s="2">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="F34" s="2">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="G34" s="2">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="H34" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="I34" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="J34" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="K34" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="L34" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="M34" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -1862,285 +1875,39 @@
         <v>3000</v>
       </c>
       <c r="B35" s="2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C35" s="2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="D35" s="2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E35" s="2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="F35" s="2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G35" s="2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H35" s="3">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I35" s="3">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="J35" s="3">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="K35" s="3">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="L35" s="3">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="M35" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>3000</v>
-      </c>
-      <c r="B36" s="2">
-        <v>50</v>
-      </c>
-      <c r="C36" s="2">
-        <v>50</v>
-      </c>
-      <c r="D36" s="2">
-        <v>50</v>
-      </c>
-      <c r="E36" s="2">
-        <v>50</v>
-      </c>
-      <c r="F36" s="2">
-        <v>50</v>
-      </c>
-      <c r="G36" s="2">
-        <v>50</v>
-      </c>
-      <c r="H36" s="3">
-        <v>50</v>
-      </c>
-      <c r="I36" s="3">
-        <v>50</v>
-      </c>
-      <c r="J36" s="3">
-        <v>50</v>
-      </c>
-      <c r="K36" s="3">
-        <v>50</v>
-      </c>
-      <c r="L36" s="3">
-        <v>50</v>
-      </c>
-      <c r="M36" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>3000</v>
-      </c>
-      <c r="B37" s="2">
-        <v>40</v>
-      </c>
-      <c r="C37" s="2">
-        <v>40</v>
-      </c>
-      <c r="D37" s="2">
-        <v>40</v>
-      </c>
-      <c r="E37" s="2">
-        <v>40</v>
-      </c>
-      <c r="F37" s="2">
-        <v>40</v>
-      </c>
-      <c r="G37" s="2">
-        <v>40</v>
-      </c>
-      <c r="H37" s="3">
-        <v>40</v>
-      </c>
-      <c r="I37" s="3">
-        <v>40</v>
-      </c>
-      <c r="J37" s="3">
-        <v>40</v>
-      </c>
-      <c r="K37" s="3">
-        <v>40</v>
-      </c>
-      <c r="L37" s="3">
-        <v>40</v>
-      </c>
-      <c r="M37" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>3000</v>
-      </c>
-      <c r="B38" s="2">
-        <v>30</v>
-      </c>
-      <c r="C38" s="2">
-        <v>30</v>
-      </c>
-      <c r="D38" s="2">
-        <v>30</v>
-      </c>
-      <c r="E38" s="2">
-        <v>30</v>
-      </c>
-      <c r="F38" s="2">
-        <v>30</v>
-      </c>
-      <c r="G38" s="2">
-        <v>30</v>
-      </c>
-      <c r="H38" s="3">
-        <v>30</v>
-      </c>
-      <c r="I38" s="3">
-        <v>30</v>
-      </c>
-      <c r="J38" s="3">
-        <v>30</v>
-      </c>
-      <c r="K38" s="3">
-        <v>30</v>
-      </c>
-      <c r="L38" s="3">
-        <v>30</v>
-      </c>
-      <c r="M38" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
-        <v>3000</v>
-      </c>
-      <c r="B39" s="2">
-        <v>20</v>
-      </c>
-      <c r="C39" s="2">
-        <v>20</v>
-      </c>
-      <c r="D39" s="2">
-        <v>20</v>
-      </c>
-      <c r="E39" s="2">
-        <v>20</v>
-      </c>
-      <c r="F39" s="2">
-        <v>20</v>
-      </c>
-      <c r="G39" s="2">
-        <v>20</v>
-      </c>
-      <c r="H39" s="3">
-        <v>20</v>
-      </c>
-      <c r="I39" s="3">
-        <v>20</v>
-      </c>
-      <c r="J39" s="3">
-        <v>20</v>
-      </c>
-      <c r="K39" s="3">
-        <v>20</v>
-      </c>
-      <c r="L39" s="3">
-        <v>20</v>
-      </c>
-      <c r="M39" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
-        <v>3000</v>
-      </c>
-      <c r="B40" s="2">
-        <v>10</v>
-      </c>
-      <c r="C40" s="2">
-        <v>10</v>
-      </c>
-      <c r="D40" s="2">
-        <v>10</v>
-      </c>
-      <c r="E40" s="2">
-        <v>10</v>
-      </c>
-      <c r="F40" s="2">
-        <v>10</v>
-      </c>
-      <c r="G40" s="2">
-        <v>10</v>
-      </c>
-      <c r="H40" s="3">
-        <v>10</v>
-      </c>
-      <c r="I40" s="3">
-        <v>10</v>
-      </c>
-      <c r="J40" s="3">
-        <v>10</v>
-      </c>
-      <c r="K40" s="3">
-        <v>10</v>
-      </c>
-      <c r="L40" s="3">
-        <v>10</v>
-      </c>
-      <c r="M40" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>3000</v>
-      </c>
-      <c r="B41" s="2">
-        <v>0</v>
-      </c>
-      <c r="C41" s="2">
-        <v>0</v>
-      </c>
-      <c r="D41" s="2">
-        <v>0</v>
-      </c>
-      <c r="E41" s="2">
-        <v>0</v>
-      </c>
-      <c r="F41" s="2">
-        <v>0</v>
-      </c>
-      <c r="G41" s="2">
-        <v>0</v>
-      </c>
-      <c r="H41" s="3">
-        <v>0</v>
-      </c>
-      <c r="I41" s="3">
-        <v>0</v>
-      </c>
-      <c r="J41" s="3">
-        <v>0</v>
-      </c>
-      <c r="K41" s="3">
-        <v>0</v>
-      </c>
-      <c r="L41" s="3">
-        <v>0</v>
-      </c>
-      <c r="M41" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>